<commit_message>
coding of basic energy projects implementation
</commit_message>
<xml_diff>
--- a/projects - calculations.xlsx
+++ b/projects - calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frac1\Documents\GitHub\SEN9120-Regional energy transition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813F577C-34C0-4355-BFE0-9EC7E95F3963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FA6809-F26D-43EC-BDB8-1DD5FF844E7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8940" yWindow="984" windowWidth="17508" windowHeight="10728" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
+    <workbookView xWindow="300" yWindow="1596" windowWidth="17508" windowHeight="10728" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Archetypes" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="179">
   <si>
     <t>type</t>
   </si>
@@ -598,6 +598,9 @@
   </si>
   <si>
     <t>solar-generating-district</t>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
@@ -4547,10 +4550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2AF2E5-58AD-468A-9D04-632533EF6A69}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4558,10 +4561,11 @@
     <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4572,10 +4576,13 @@
         <v>166</v>
       </c>
       <c r="D1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -4586,116 +4593,141 @@
       <c r="C2">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B3" s="1">
-        <f>'Offshore wind'!I24*C3</f>
-        <v>157440000</v>
+        <f>'Solar Photovoltaic'!B41*Archetypes!C3</f>
+        <v>10885499.999999998</v>
       </c>
       <c r="C3">
-        <v>120</v>
-      </c>
-      <c r="D3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="2">
+        <f>'Onshore wind'!B34*Archetypes!C4</f>
+        <v>4100000</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="1">
-        <f>'Offshore wind'!I24*C4</f>
+      <c r="B5" s="1">
+        <f>'Offshore wind'!I24*C5</f>
         <v>164000000</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>125</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>127</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="1">
-        <f>'Solar Photovoltaic'!B41*Archetypes!C5</f>
-        <v>10885499.999999998</v>
-      </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B6" s="1">
         <f>'Solar Photovoltaic'!B41*Archetypes!C6</f>
+        <v>21045299.999999996</v>
+      </c>
+      <c r="C6">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="2">
+        <f>'Onshore wind'!B34*Archetypes!C7</f>
+        <v>7380000</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="1">
+        <f>'Offshore wind'!I24*C8</f>
+        <v>157440000</v>
+      </c>
+      <c r="C8">
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="1">
+        <f>'Solar Photovoltaic'!B41*Archetypes!C9</f>
         <v>34107899.999999993</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B7" s="1">
-        <f>'Solar Photovoltaic'!B41*Archetypes!C7</f>
-        <v>21045299.999999996</v>
-      </c>
-      <c r="C7">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0.25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B9" s="2">
-        <f>'Onshore wind'!B34*Archetypes!C9</f>
-        <v>4100000</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -4706,23 +4738,28 @@
       <c r="C10">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B11" s="2">
-        <f>'Onshore wind'!B34*Archetypes!C11</f>
-        <v>7380000</v>
+        <v>177</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>125</v>
+        <v>0.25</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>